<commit_message>
float_format='%.2f' when writing tidally_corrected.csv
</commit_message>
<xml_diff>
--- a/data/nzd0013/nzd0013.xlsx
+++ b/data/nzd0013/nzd0013.xlsx
@@ -499,7 +499,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>419.595</v>
+        <v>419.6</v>
       </c>
       <c r="C4" t="n">
         <v>377.73</v>
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>431.565</v>
+        <v>431.56</v>
       </c>
       <c r="C6" t="n">
         <v>392.11</v>
@@ -553,7 +553,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>392.445</v>
+        <v>392.44</v>
       </c>
       <c r="C7" t="n">
         <v>386.63</v>
@@ -589,7 +589,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>385.875</v>
+        <v>385.88</v>
       </c>
       <c r="C9" t="n">
         <v>388.22</v>
@@ -643,7 +643,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>370.835</v>
+        <v>370.83</v>
       </c>
       <c r="C12" t="n">
         <v>378.54</v>
@@ -661,7 +661,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>376.205</v>
+        <v>376.2</v>
       </c>
       <c r="C13" t="n">
         <v>388.68</v>
@@ -749,7 +749,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>379.735</v>
+        <v>379.74</v>
       </c>
       <c r="C18" t="n">
         <v>389.56</v>
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>390.215</v>
+        <v>390.21</v>
       </c>
       <c r="C19" t="n">
         <v>370.72</v>
@@ -785,7 +785,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>386.365</v>
+        <v>386.37</v>
       </c>
       <c r="C20" t="n">
         <v>375.43</v>
@@ -803,7 +803,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>392.885</v>
+        <v>392.88</v>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
@@ -819,7 +819,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>422.975</v>
+        <v>422.98</v>
       </c>
       <c r="C22" t="n">
         <v>386.29</v>
@@ -855,10 +855,10 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>376.715</v>
+        <v>376.71</v>
       </c>
       <c r="C24" t="n">
-        <v>392.0100000000001</v>
+        <v>392.01</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -873,7 +873,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>381.355</v>
+        <v>381.36</v>
       </c>
       <c r="C25" t="n">
         <v>388.74</v>
@@ -925,7 +925,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>374.105</v>
+        <v>374.11</v>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
@@ -959,7 +959,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>380.235</v>
+        <v>380.24</v>
       </c>
       <c r="C30" t="n">
         <v>395.8</v>
@@ -1047,7 +1047,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>418.865</v>
+        <v>418.87</v>
       </c>
       <c r="C35" t="n">
         <v>375.15</v>
@@ -1101,7 +1101,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>410.165</v>
+        <v>410.17</v>
       </c>
       <c r="C38" t="n">
         <v>377.55</v>
@@ -1137,7 +1137,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>431.935</v>
+        <v>431.94</v>
       </c>
       <c r="C40" t="n">
         <v>381.11</v>
@@ -1171,7 +1171,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>438.695</v>
+        <v>438.69</v>
       </c>
       <c r="C42" t="n">
         <v>381.8</v>
@@ -1255,7 +1255,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>442.965</v>
+        <v>442.96</v>
       </c>
       <c r="C47" t="n">
         <v>387.07</v>
@@ -1307,7 +1307,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>423.625</v>
+        <v>423.62</v>
       </c>
       <c r="C50" t="n">
         <v>380.99</v>
@@ -1359,7 +1359,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>441.645</v>
+        <v>441.64</v>
       </c>
       <c r="C53" t="n">
         <v>400.21</v>
@@ -1429,7 +1429,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>404.225</v>
+        <v>404.23</v>
       </c>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr">
@@ -1445,10 +1445,10 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>371.965</v>
+        <v>371.96</v>
       </c>
       <c r="C58" t="n">
-        <v>385.3200000000001</v>
+        <v>385.32</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -1533,7 +1533,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>401.535</v>
+        <v>401.54</v>
       </c>
       <c r="C63" t="n">
         <v>366.3</v>
@@ -1569,7 +1569,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>373.975</v>
+        <v>373.98</v>
       </c>
       <c r="C65" t="n">
         <v>374.64</v>
@@ -1639,7 +1639,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>360.175</v>
+        <v>360.18</v>
       </c>
       <c r="C69" t="n">
         <v>365.7</v>
@@ -1691,7 +1691,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>360.245</v>
+        <v>360.25</v>
       </c>
       <c r="C72" t="n">
         <v>366.84</v>
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>378.915</v>
+        <v>378.92</v>
       </c>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr">
@@ -1773,7 +1773,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>427.085</v>
+        <v>427.08</v>
       </c>
       <c r="C77" t="n">
         <v>377.29</v>
@@ -1877,7 +1877,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>447.775</v>
+        <v>447.77</v>
       </c>
       <c r="C83" t="n">
         <v>408.01</v>
@@ -1913,10 +1913,10 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>448.675</v>
+        <v>448.68</v>
       </c>
       <c r="C85" t="n">
-        <v>391.9500000000001</v>
+        <v>391.95</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -1931,7 +1931,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>431.795</v>
+        <v>431.8</v>
       </c>
       <c r="C86" t="n">
         <v>382.55</v>
@@ -1949,7 +1949,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>405.925</v>
+        <v>405.93</v>
       </c>
       <c r="C87" t="n">
         <v>391.29</v>
@@ -1967,7 +1967,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>379.305</v>
+        <v>379.31</v>
       </c>
       <c r="C88" t="n">
         <v>376.06</v>
@@ -2003,7 +2003,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>385.205</v>
+        <v>385.2</v>
       </c>
       <c r="C90" t="n">
         <v>367.81</v>
@@ -2021,7 +2021,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>368.995</v>
+        <v>369</v>
       </c>
       <c r="C91" t="n">
         <v>375.23</v>
@@ -2039,7 +2039,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>363.905</v>
+        <v>363.9</v>
       </c>
       <c r="C92" t="n">
         <v>379.79</v>
@@ -2091,7 +2091,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>385.885</v>
+        <v>385.88</v>
       </c>
       <c r="C95" t="n">
         <v>400.84</v>
@@ -2109,7 +2109,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>371.755</v>
+        <v>371.75</v>
       </c>
       <c r="C96" t="inlineStr"/>
       <c r="D96" t="inlineStr">
@@ -2177,7 +2177,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>368.365</v>
+        <v>368.37</v>
       </c>
       <c r="C100" t="n">
         <v>380.47</v>
@@ -2213,7 +2213,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>369.555</v>
+        <v>369.56</v>
       </c>
       <c r="C102" t="inlineStr"/>
       <c r="D102" t="inlineStr">
@@ -2229,7 +2229,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>373.145</v>
+        <v>373.14</v>
       </c>
       <c r="C103" t="n">
         <v>390.04</v>
@@ -2317,7 +2317,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>437.235</v>
+        <v>437.24</v>
       </c>
       <c r="C108" t="n">
         <v>380.5</v>
@@ -2335,7 +2335,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>428.095</v>
+        <v>428.1</v>
       </c>
       <c r="C109" t="n">
         <v>390.52</v>
@@ -2353,7 +2353,7 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>406.295</v>
+        <v>406.3</v>
       </c>
       <c r="C110" t="n">
         <v>382.48</v>
@@ -2405,7 +2405,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>376.865</v>
+        <v>376.87</v>
       </c>
       <c r="C113" t="n">
         <v>382.94</v>
@@ -2423,7 +2423,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>447.365</v>
+        <v>447.37</v>
       </c>
       <c r="C114" t="n">
         <v>396.16</v>
@@ -2441,7 +2441,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>431.845</v>
+        <v>431.85</v>
       </c>
       <c r="C115" t="n">
         <v>384.08</v>
@@ -2459,7 +2459,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>416.785</v>
+        <v>416.79</v>
       </c>
       <c r="C116" t="n">
         <v>375.01</v>
@@ -2495,7 +2495,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>406.005</v>
+        <v>406</v>
       </c>
       <c r="C118" t="n">
         <v>372.38</v>
@@ -2513,7 +2513,7 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>379.425</v>
+        <v>379.43</v>
       </c>
       <c r="C119" t="n">
         <v>386.8</v>
@@ -2549,7 +2549,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>375.315</v>
+        <v>375.31</v>
       </c>
       <c r="C121" t="inlineStr"/>
       <c r="D121" t="inlineStr">
@@ -2565,7 +2565,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>380.125</v>
+        <v>380.12</v>
       </c>
       <c r="C122" t="n">
         <v>381.41</v>
@@ -2583,7 +2583,7 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>409.855</v>
+        <v>409.86</v>
       </c>
       <c r="C123" t="n">
         <v>369.13</v>
@@ -2637,7 +2637,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>379.255</v>
+        <v>379.25</v>
       </c>
       <c r="C126" t="n">
         <v>384.63</v>
@@ -2655,7 +2655,7 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>350.465</v>
+        <v>350.46</v>
       </c>
       <c r="C127" t="n">
         <v>373.18</v>
@@ -2707,7 +2707,7 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>416.785</v>
+        <v>416.79</v>
       </c>
       <c r="C130" t="n">
         <v>377.76</v>
@@ -2725,7 +2725,7 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>415.625</v>
+        <v>415.62</v>
       </c>
       <c r="C131" t="n">
         <v>381.81</v>
@@ -2797,7 +2797,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>375.095</v>
+        <v>375.1</v>
       </c>
       <c r="C135" t="n">
         <v>389.74</v>
@@ -2815,7 +2815,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>373.665</v>
+        <v>373.67</v>
       </c>
       <c r="C136" t="n">
         <v>383.56</v>
@@ -2923,7 +2923,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>368.265</v>
+        <v>368.26</v>
       </c>
       <c r="C142" t="n">
         <v>387.53</v>
@@ -2977,7 +2977,7 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>367.485</v>
+        <v>367.49</v>
       </c>
       <c r="C145" t="inlineStr"/>
       <c r="D145" t="inlineStr">
@@ -3079,7 +3079,7 @@
         </is>
       </c>
       <c r="B151" t="n">
-        <v>376.845</v>
+        <v>376.85</v>
       </c>
       <c r="C151" t="n">
         <v>390.79</v>
@@ -3115,7 +3115,7 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>348.815</v>
+        <v>348.81</v>
       </c>
       <c r="C153" t="n">
         <v>374.62</v>
@@ -3133,7 +3133,7 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>363.925</v>
+        <v>363.93</v>
       </c>
       <c r="C154" t="n">
         <v>393.91</v>
@@ -3169,7 +3169,7 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>361.535</v>
+        <v>361.54</v>
       </c>
       <c r="C156" t="n">
         <v>377.99</v>
@@ -3239,7 +3239,7 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>353.315</v>
+        <v>353.31</v>
       </c>
       <c r="C160" t="n">
         <v>386.32</v>
@@ -3307,7 +3307,7 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>367.305</v>
+        <v>367.31</v>
       </c>
       <c r="C164" t="n">
         <v>384.93</v>
@@ -3325,7 +3325,7 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>420.705</v>
+        <v>420.7</v>
       </c>
       <c r="C165" t="n">
         <v>381.96</v>
@@ -3346,7 +3346,7 @@
         <v>416.23</v>
       </c>
       <c r="C166" t="n">
-        <v>385.5100000000001</v>
+        <v>385.51</v>
       </c>
       <c r="D166" t="inlineStr">
         <is>
@@ -3361,7 +3361,7 @@
         </is>
       </c>
       <c r="B167" t="n">
-        <v>404.935</v>
+        <v>404.94</v>
       </c>
       <c r="C167" t="n">
         <v>388</v>
@@ -3379,7 +3379,7 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>414.995</v>
+        <v>415</v>
       </c>
       <c r="C168" t="n">
         <v>378.68</v>
@@ -3431,7 +3431,7 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>366.825</v>
+        <v>366.82</v>
       </c>
       <c r="C171" t="n">
         <v>376.56</v>
@@ -3467,7 +3467,7 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>383.945</v>
+        <v>383.94</v>
       </c>
       <c r="C173" t="n">
         <v>390.21</v>
@@ -3555,7 +3555,7 @@
         </is>
       </c>
       <c r="B178" t="n">
-        <v>442.145</v>
+        <v>442.14</v>
       </c>
       <c r="C178" t="n">
         <v>392.05</v>
@@ -3573,7 +3573,7 @@
         </is>
       </c>
       <c r="B179" t="n">
-        <v>441.535</v>
+        <v>441.54</v>
       </c>
       <c r="C179" t="n">
         <v>388.19</v>
@@ -3609,7 +3609,7 @@
         </is>
       </c>
       <c r="B181" t="n">
-        <v>410.325</v>
+        <v>410.32</v>
       </c>
       <c r="C181" t="n">
         <v>380.08</v>
@@ -3627,7 +3627,7 @@
         </is>
       </c>
       <c r="B182" t="n">
-        <v>418.725</v>
+        <v>418.73</v>
       </c>
       <c r="C182" t="n">
         <v>389.03</v>
@@ -3645,7 +3645,7 @@
         </is>
       </c>
       <c r="B183" t="n">
-        <v>415.585</v>
+        <v>415.58</v>
       </c>
       <c r="C183" t="n">
         <v>385.27</v>
@@ -3789,7 +3789,7 @@
         </is>
       </c>
       <c r="B191" t="n">
-        <v>380.985</v>
+        <v>380.99</v>
       </c>
       <c r="C191" t="n">
         <v>389.69</v>
@@ -3807,7 +3807,7 @@
         </is>
       </c>
       <c r="B192" t="n">
-        <v>371.555</v>
+        <v>371.56</v>
       </c>
       <c r="C192" t="n">
         <v>376.9</v>
@@ -3877,7 +3877,7 @@
         </is>
       </c>
       <c r="B196" t="n">
-        <v>379.315</v>
+        <v>379.31</v>
       </c>
       <c r="C196" t="n">
         <v>386.14</v>
@@ -3995,7 +3995,7 @@
         </is>
       </c>
       <c r="B203" t="n">
-        <v>426.535</v>
+        <v>426.54</v>
       </c>
       <c r="C203" t="n">
         <v>362.69</v>
@@ -4031,7 +4031,7 @@
         </is>
       </c>
       <c r="B205" t="n">
-        <v>370.085</v>
+        <v>370.08</v>
       </c>
       <c r="C205" t="n">
         <v>391.12</v>
@@ -4101,7 +4101,7 @@
         </is>
       </c>
       <c r="B209" t="n">
-        <v>421.195</v>
+        <v>421.19</v>
       </c>
       <c r="C209" t="n">
         <v>392.66</v>
@@ -7024,7 +7024,7 @@
         <v>0.08690000000000001</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.7059748193353359</v>
+        <v>-0.705982616655231</v>
       </c>
       <c r="J2" t="n">
         <v>208</v>
@@ -7033,19 +7033,19 @@
         <v>174</v>
       </c>
       <c r="L2" t="n">
-        <v>0.03988320031284076</v>
+        <v>0.03988370355105508</v>
       </c>
       <c r="M2" t="n">
-        <v>23.81253677408011</v>
+        <v>23.81279288939012</v>
       </c>
       <c r="N2" t="n">
-        <v>742.9477424150858</v>
+        <v>742.9543899907881</v>
       </c>
       <c r="O2" t="n">
-        <v>27.25706775159584</v>
+        <v>27.25718969356137</v>
       </c>
       <c r="P2" t="n">
-        <v>403.1753720075986</v>
+        <v>403.1758040828076</v>
       </c>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr">
@@ -7102,7 +7102,7 @@
         <v>0.0517</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1361318337345997</v>
+        <v>0.1361318337345998</v>
       </c>
       <c r="J3" t="n">
         <v>208</v>
@@ -7111,10 +7111,10 @@
         <v>197</v>
       </c>
       <c r="L3" t="n">
-        <v>0.01566913003713066</v>
+        <v>0.01566913003713033</v>
       </c>
       <c r="M3" t="n">
-        <v>6.75354383939097</v>
+        <v>6.753543839390966</v>
       </c>
       <c r="N3" t="n">
         <v>73.3131513207571</v>
@@ -7239,7 +7239,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>-34.72282043246782,173.09217283317156</t>
+          <t>-34.72282041961203,173.09217288551477</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -7283,7 +7283,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>-34.722789655599094,173.09229814279226</t>
+          <t>-34.72278966845495,173.09229809044908</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -7305,7 +7305,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>-34.72289023917352,173.09188860925056</t>
+          <t>-34.72289025202922,173.09188855690724</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -7349,7 +7349,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>-34.722907131525325,173.09181983013025</t>
+          <t>-34.72290711866965,173.09181988247357</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -7415,7 +7415,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>-34.72294580123769,173.09166238132303</t>
+          <t>-34.72294581409329,173.09166232897965</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -7437,7 +7437,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>-34.72293199432253,173.09171859810152</t>
+          <t>-34.72293200717814,173.09171854575817</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -7543,7 +7543,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>-34.72292291825429,173.09175555250994</t>
+          <t>-34.722922905398654,173.0917556048533</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -7565,7 +7565,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>-34.72289597280718,173.0918652641337</t>
+          <t>-34.722895985662866,173.0918652117904</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -7587,7 +7587,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>-34.72290587167088,173.0918249597764</t>
+          <t>-34.722905858815224,173.09182501211973</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -7609,7 +7609,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>-34.72288910787309,173.09189321546157</t>
+          <t>-34.722889120728794,173.09189316311827</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
@@ -7627,7 +7627,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>-34.722811741936496,173.09220821718415</t>
+          <t>-34.72281172908067,173.0922082695274</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -7671,7 +7671,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>-34.72293068304991,173.09172393712421</t>
+          <t>-34.722930695905525,173.09172388478086</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -7693,7 +7693,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>-34.72291875302942,173.0917725117542</t>
+          <t>-34.72291874017379,173.0917725640975</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -7755,7 +7755,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>-34.72293739367791,173.09169661388873</t>
+          <t>-34.7229373808223,173.09169666623208</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
@@ -7795,7 +7795,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>-34.7229216326913,173.09176078684476</t>
+          <t>-34.722921619835674,173.0917608391881</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -7901,7 +7901,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>-34.72282230941554,173.09216519106135</t>
+          <t>-34.72282229655974,173.09216524340457</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -7967,7 +7967,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>-34.72284467848165,173.09207411383085</t>
+          <t>-34.722844665625885,173.0920741661741</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -8011,7 +8011,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>-34.72278870426525,173.09230201618757</t>
+          <t>-34.722788691409384,173.09230206853073</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -8051,7 +8051,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>-34.72277132311728,173.09237278415114</t>
+          <t>-34.722771335973164,173.09237273180796</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -8149,7 +8149,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>-34.72276034417569,173.09241748520157</t>
+          <t>-34.72276035703161,173.0924174328584</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -8211,7 +8211,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>-34.72281007067928,173.09221502180114</t>
+          <t>-34.722810083535116,173.09221496945793</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -8273,7 +8273,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>-34.72276373813596,173.09240366661112</t>
+          <t>-34.722763750991874,173.09240361426797</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -8357,7 +8357,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>-34.72285995111526,173.0920119300383</t>
+          <t>-34.72285993825952,173.09201198238154</t>
         </is>
       </c>
       <c r="C57" t="inlineStr"/>
@@ -8375,7 +8375,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>-34.72294289587408,173.09167421092602</t>
+          <t>-34.722942908729685,173.09167415858266</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -8481,7 +8481,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>-34.722866867499505,173.09198376935703</t>
+          <t>-34.72286685464377,173.0919838217003</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -8525,7 +8525,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>-34.72293772792359,173.09169525296116</t>
+          <t>-34.722937715067985,173.09169530530454</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -8609,7 +8609,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>-34.72297320930156,173.09155078520442</t>
+          <t>-34.72297319644601,173.09155083754783</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -8671,7 +8671,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>-34.72297302932398,173.09155151801218</t>
+          <t>-34.722973016468444,173.0915515703556</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -8711,7 +8711,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>-34.72292502657708,173.0917469682005</t>
+          <t>-34.722925013721465,173.09174702054383</t>
         </is>
       </c>
       <c r="C74" t="inlineStr"/>
@@ -8765,7 +8765,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>-34.72280117444224,173.09225124329598</t>
+          <t>-34.722801187298096,173.09225119095282</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -8889,7 +8889,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>-34.722747976776894,173.09246783929802</t>
+          <t>-34.72274798963282,173.0924677869549</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -8933,7 +8933,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>-34.72274566270827,173.0924772610608</t>
+          <t>-34.72274564985234,173.09247731340392</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -8955,7 +8955,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>-34.72278906422941,173.09230055057853</t>
+          <t>-34.72278905137355,173.09230060292174</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -8977,7 +8977,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>-34.72285558016275,173.09202972674893</t>
+          <t>-34.722855567307015,173.0920297790922</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -8999,7 +8999,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>-34.722924023838274,173.09175105098188</t>
+          <t>-34.72292401098264,173.09175110332524</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -9043,7 +9043,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>-34.72290885418305,173.09181281612402</t>
+          <t>-34.72290886703872,173.09181276378067</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -9065,7 +9065,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>-34.72295053209279,173.09164311895884</t>
+          <t>-34.72295051923721,173.09164317130222</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -9087,7 +9087,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>-34.72296361906194,173.09158983338565</t>
+          <t>-34.722963631917494,173.09158978104225</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -9149,7 +9149,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>-34.72290710581401,173.0918199348169</t>
+          <t>-34.72290711866965,173.09181988247357</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -9171,7 +9171,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>-34.72294343580899,173.09167201250432</t>
+          <t>-34.72294344866459,173.09167196016094</t>
         </is>
       </c>
       <c r="C96" t="inlineStr"/>
@@ -9251,7 +9251,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>-34.72295215189574,173.0916365236924</t>
+          <t>-34.72295213904017,173.09163657603577</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -9295,7 +9295,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>-34.722949092267655,173.09164898141776</t>
+          <t>-34.72294907941206,173.09164903376114</t>
         </is>
       </c>
       <c r="C102" t="inlineStr"/>
@@ -9313,7 +9313,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>-34.72293986195334,173.09168656396187</t>
+          <t>-34.722939874808944,173.09168651161852</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -9419,7 +9419,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>-34.72277507703734,173.0923574999485</t>
+          <t>-34.722775064181434,173.09235755229165</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -9441,7 +9441,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>-34.72279857756176,173.09226181662106</t>
+          <t>-34.722798564705926,173.09226186896427</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -9463,7 +9463,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>-34.722854628837446,173.09203360015042</t>
+          <t>-34.7228546159817,173.09203365249368</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -9525,7 +9525,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>-34.72293029738143,173.09172550742497</t>
+          <t>-34.72293028452582,173.09172555976832</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -9547,7 +9547,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>-34.72274903096346,173.0924635471615</t>
+          <t>-34.72274901810753,173.0924635995046</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -9569,7 +9569,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>-34.72278893567079,173.09230107401032</t>
+          <t>-34.722788922814914,173.09230112635353</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -9591,7 +9591,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>-34.72282765742834,173.09214341627967</t>
+          <t>-34.72282764457257,173.0921434686229</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -9635,7 +9635,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>-34.722855374470804,173.09203056424116</t>
+          <t>-34.72285538732656,173.0920305118979</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -9657,7 +9657,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>-34.72292371530321,173.0917523072223</t>
+          <t>-34.722923702447595,173.09175235956562</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -9701,7 +9701,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>-34.722934282621246,173.0917092809831</t>
+          <t>-34.72293429547685,173.09170922863976</t>
         </is>
       </c>
       <c r="C121" t="inlineStr"/>
@@ -9719,7 +9719,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>-34.72292191551518,173.0917596352911</t>
+          <t>-34.7229219283708,173.09175958294776</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -9741,7 +9741,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>-34.72284547553908,173.09207086854929</t>
+          <t>-34.7228454626833,173.09207092089255</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -9807,7 +9807,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>-34.722924152394526,173.09175052754838</t>
+          <t>-34.722924165250156,173.09175047520503</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -9829,7 +9829,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>-34.72299817471916,173.09144913426658</t>
+          <t>-34.72299818757466,173.09144908192314</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -9891,7 +9891,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>-34.72282765742834,173.09214341627967</t>
+          <t>-34.72282764457257,173.0921434686229</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -9913,7 +9913,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>-34.72283063997226,173.09213127265022</t>
+          <t>-34.72283065282805,173.09213122030698</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -10001,7 +10001,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>-34.722934848268004,173.0917069778751</t>
+          <t>-34.72293483541241,173.0917070302185</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -10023,7 +10023,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>-34.72293852497092,173.09169200767232</t>
+          <t>-34.72293851211533,173.09169206001567</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -10155,7 +10155,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>-34.72295240900728,173.09163547682462</t>
+          <t>-34.72295242186286,173.09163542448124</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -10221,7 +10221,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>-34.722954414477044,173.0916273112562</t>
+          <t>-34.722954401621465,173.09162736359957</t>
         </is>
       </c>
       <c r="C145" t="inlineStr"/>
@@ -10341,7 +10341,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>-34.72293034880391,173.09172529805153</t>
+          <t>-34.722930335948284,173.09172535039488</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -10385,7 +10385,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>-34.72300241703196,173.09143186092913</t>
+          <t>-34.723002429887444,173.0914318085857</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -10407,7 +10407,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>-34.722963567639724,173.09159004275924</t>
+          <t>-34.72296355478416,173.09159009510265</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -10451,7 +10451,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>-34.72296971259365,173.091565022612</t>
+          <t>-34.7229696997381,173.0915650749554</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -10535,7 +10535,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>-34.72299084708221,173.09147897002708</t>
+          <t>-34.722990859937724,173.09147891768365</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -10615,7 +10615,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>-34.722954877277665,173.09162542689418</t>
+          <t>-34.7229548644221,173.09162547923756</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -10637,7 +10637,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>-34.72281757847789,173.09218445336586</t>
+          <t>-34.7228175913337,173.09218440102265</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -10681,7 +10681,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>-34.72285812560012,173.09201936278237</t>
+          <t>-34.722858112744376,173.09201941512566</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -10703,7 +10703,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>-34.72283225980163,173.0921246774028</t>
+          <t>-34.72283224694585,173.09212472974605</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -10765,7 +10765,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>-34.72295611141255,173.0916204019287</t>
+          <t>-34.72295612426812,173.09162034958533</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -10809,7 +10809,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>-34.72291209380697,173.091799625604</t>
+          <t>-34.72291210666262,173.0917995732607</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -10915,7 +10915,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>-34.72276245254513,173.0924089009258</t>
+          <t>-34.72276246540105,173.09240884858266</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -10937,7 +10937,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>-34.722764020965926,173.09240251506188</t>
+          <t>-34.722764008110005,173.092402567405</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -10981,7 +10981,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>-34.72284426709714,173.0920757888148</t>
+          <t>-34.72284427995291,173.09207573647157</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -11003,7 +11003,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>-34.72282266937807,173.09216372545114</t>
+          <t>-34.722822656522254,173.09216377779435</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -11025,7 +11025,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>-34.72283074281858,173.09213085390434</t>
+          <t>-34.72283075567437,173.09213080156113</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -11201,7 +11201,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>-34.722919704346424,173.0917686383467</t>
+          <t>-34.72291969149078,173.09176869069003</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
@@ -11223,7 +11223,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>-34.7229439500327,173.09166991876927</t>
+          <t>-34.72294393717711,173.09166997111265</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -11307,7 +11307,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>-34.722923998127015,173.0917511556686</t>
+          <t>-34.72292401098264,173.09175110332524</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -11445,7 +11445,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>-34.7228025885847,173.09224548554442</t>
+          <t>-34.72280257572885,173.09224553788764</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
@@ -11489,7 +11489,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>-34.72294772957573,173.09165452981617</t>
+          <t>-34.722947742431316,173.0916544774728</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
@@ -11573,7 +11573,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>-34.72281631860812,173.09218958300093</t>
+          <t>-34.722816331463925,173.09218953065772</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">

</xml_diff>